<commit_message>
0.22.15 - tech tree update
</commit_message>
<xml_diff>
--- a/anw/Data/tech.xlsx
+++ b/anw/Data/tech.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\development\cosmica\anw\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0863374D-5E30-4FD6-B347-3D23E8F56171}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F107E17-12F0-4C5D-BDAD-052A7B3C1916}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tech.csv" sheetId="1" r:id="rId1"/>
@@ -2059,33 +2059,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="H77" sqref="H77"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="3" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2610,7 +2610,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3170,7 +3170,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3800,7 +3800,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4150,7 +4150,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -4220,7 +4220,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -4325,7 +4325,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -4430,7 +4430,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -4535,7 +4535,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -4675,7 +4675,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>100</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>101</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>102</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>103</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>104</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>105</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>106</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>107</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>108</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>109</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>110</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>111</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>112</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>113</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>114</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>115</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>116</v>
       </c>
@@ -5270,7 +5270,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>117</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>118</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>119</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>120</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>121</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>122</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>123</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>124</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>125</v>
       </c>
@@ -5585,7 +5585,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>126</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>127</v>
       </c>
@@ -5655,7 +5655,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>128</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>129</v>
       </c>
@@ -5725,7 +5725,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>130</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>131</v>
       </c>
@@ -5795,7 +5795,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>132</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>133</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>134</v>
       </c>
@@ -5900,7 +5900,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>135</v>
       </c>
@@ -5935,7 +5935,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>136</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>137</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>138</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>139</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>140</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>141</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>142</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>143</v>
       </c>
@@ -6215,7 +6215,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>144</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>145</v>
       </c>
@@ -6285,7 +6285,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>146</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>147</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>148</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>149</v>
       </c>
@@ -6425,7 +6425,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>150</v>
       </c>
@@ -6460,7 +6460,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>151</v>
       </c>
@@ -6495,7 +6495,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>152</v>
       </c>
@@ -6530,7 +6530,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>153</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>154</v>
       </c>
@@ -6600,7 +6600,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>155</v>
       </c>
@@ -6635,7 +6635,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>156</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>157</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>158</v>
       </c>
@@ -6740,7 +6740,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>159</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>160</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>161</v>
       </c>
@@ -6845,7 +6845,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>162</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>163</v>
       </c>
@@ -6915,7 +6915,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>164</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>165</v>
       </c>
@@ -6985,7 +6985,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>166</v>
       </c>
@@ -7020,7 +7020,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>167</v>
       </c>
@@ -7055,7 +7055,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>168</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>169</v>
       </c>
@@ -7125,7 +7125,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>170</v>
       </c>
@@ -7160,7 +7160,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>200</v>
       </c>
@@ -7195,7 +7195,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>201</v>
       </c>
@@ -7230,7 +7230,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>202</v>
       </c>
@@ -7265,7 +7265,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>203</v>
       </c>
@@ -7300,7 +7300,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>204</v>
       </c>
@@ -7335,7 +7335,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>205</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>206</v>
       </c>
@@ -7405,7 +7405,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>207</v>
       </c>
@@ -7440,7 +7440,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>208</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>209</v>
       </c>
@@ -7510,7 +7510,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>210</v>
       </c>
@@ -7545,7 +7545,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>211</v>
       </c>
@@ -7580,7 +7580,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>212</v>
       </c>
@@ -7615,7 +7615,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>213</v>
       </c>
@@ -7650,7 +7650,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>214</v>
       </c>
@@ -7685,7 +7685,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>215</v>
       </c>
@@ -7720,7 +7720,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>216</v>
       </c>
@@ -7755,7 +7755,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>217</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>218</v>
       </c>
@@ -7825,7 +7825,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>219</v>
       </c>
@@ -7860,7 +7860,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>220</v>
       </c>
@@ -7895,7 +7895,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>221</v>
       </c>
@@ -7930,7 +7930,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>222</v>
       </c>
@@ -7965,7 +7965,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>223</v>
       </c>
@@ -8000,7 +8000,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>224</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>225</v>
       </c>
@@ -8070,7 +8070,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>226</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>227</v>
       </c>
@@ -8140,7 +8140,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>228</v>
       </c>
@@ -8175,7 +8175,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>229</v>
       </c>
@@ -8210,7 +8210,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>230</v>
       </c>
@@ -8245,7 +8245,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>231</v>
       </c>
@@ -8280,7 +8280,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>232</v>
       </c>
@@ -8315,7 +8315,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>233</v>
       </c>
@@ -8350,7 +8350,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>234</v>
       </c>
@@ -8385,7 +8385,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>235</v>
       </c>
@@ -8420,7 +8420,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>236</v>
       </c>
@@ -8455,7 +8455,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>237</v>
       </c>
@@ -8490,7 +8490,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>238</v>
       </c>
@@ -8525,7 +8525,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>239</v>
       </c>
@@ -8560,7 +8560,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>240</v>
       </c>
@@ -8595,7 +8595,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>241</v>
       </c>
@@ -8630,7 +8630,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>242</v>
       </c>
@@ -8665,7 +8665,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>243</v>
       </c>
@@ -8700,7 +8700,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>244</v>
       </c>
@@ -8735,7 +8735,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>245</v>
       </c>
@@ -8770,7 +8770,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>246</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>247</v>
       </c>
@@ -8840,7 +8840,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>248</v>
       </c>
@@ -8875,7 +8875,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>249</v>
       </c>
@@ -8910,7 +8910,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>250</v>
       </c>
@@ -8945,7 +8945,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>251</v>
       </c>
@@ -8980,7 +8980,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>252</v>
       </c>
@@ -9015,7 +9015,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>253</v>
       </c>
@@ -9050,7 +9050,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>254</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>255</v>
       </c>
@@ -9120,7 +9120,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>256</v>
       </c>
@@ -9155,7 +9155,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>257</v>
       </c>
@@ -9190,7 +9190,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>258</v>
       </c>
@@ -9201,7 +9201,7 @@
         <v>21</v>
       </c>
       <c r="D206">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E206">
         <v>0</v>
@@ -9225,7 +9225,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>259</v>
       </c>
@@ -9260,7 +9260,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>260</v>
       </c>
@@ -9295,7 +9295,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>261</v>
       </c>
@@ -9330,7 +9330,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>262</v>
       </c>
@@ -9365,7 +9365,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>263</v>
       </c>
@@ -9400,7 +9400,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>264</v>
       </c>
@@ -9435,7 +9435,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>265</v>
       </c>
@@ -9470,7 +9470,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>266</v>
       </c>
@@ -9505,7 +9505,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>267</v>
       </c>
@@ -9540,7 +9540,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>268</v>
       </c>
@@ -9575,7 +9575,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>269</v>
       </c>
@@ -9610,7 +9610,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>270</v>
       </c>
@@ -9645,7 +9645,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>271</v>
       </c>
@@ -9680,7 +9680,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>272</v>
       </c>
@@ -9715,7 +9715,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>273</v>
       </c>

</xml_diff>